<commit_message>
Tested sprint 3 in Mozilla
</commit_message>
<xml_diff>
--- a/Test-cases/Sprint 3.xlsx
+++ b/Test-cases/Sprint 3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="420" windowWidth="27660" windowHeight="16180" tabRatio="764" activeTab="5"/>
+    <workbookView xWindow="4215" yWindow="420" windowWidth="19440" windowHeight="12240" tabRatio="764" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Employee view customer Info" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="41">
   <si>
     <t>Purpose :</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Test Result :</t>
   </si>
   <si>
-    <t>Tested</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>1. click on order</t>
   </si>
   <si>
-    <t>NOT OK</t>
-  </si>
-  <si>
     <t>Test205</t>
   </si>
   <si>
@@ -147,13 +141,19 @@
   </si>
   <si>
     <t>used to work but does not work anymore</t>
+  </si>
+  <si>
+    <t>1. Tested(Chrome)</t>
+  </si>
+  <si>
+    <t>2. Tested(Mozilla)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,13 +190,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -213,7 +206,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,11 +230,6 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -252,15 +240,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -282,18 +269,17 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+  <cellStyles count="7">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -593,125 +579,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C13" sqref="C13:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="51.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="C5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="C7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="C8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>5</v>
+      <c r="C13" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -735,125 +729,133 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C13" sqref="C13:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="51.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="C3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="C5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="C7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="C8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>5</v>
+      <c r="C13" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -880,119 +882,127 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C12" sqref="C12:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="51.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="C3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="C7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="C9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>5</v>
+      <c r="C12" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" ht="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D18" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1018,126 +1028,134 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C13" sqref="C13:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="51.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="C3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" ht="24">
+      <c r="C7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="15">
+      <c r="C10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="C13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1160,133 +1178,141 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="51.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="C3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="C4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" ht="25.5" customHeight="1">
+      <c r="C7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" ht="25.5" customHeight="1">
+      <c r="C8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="25.5" customHeight="1">
+      <c r="C9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="C11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>5</v>
+      <c r="C14" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1311,117 +1337,125 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="51.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="C3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="C4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" ht="25.5" customHeight="1">
+      <c r="C7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="C9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>6</v>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>